<commit_message>
last 6 months work
</commit_message>
<xml_diff>
--- a/adm/2017HandinStatistics.xlsx
+++ b/adm/2017HandinStatistics.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3400" yWindow="460" windowWidth="11120" windowHeight="12280" tabRatio="500"/>
+    <workbookView xWindow="1840" yWindow="2740" windowWidth="11120" windowHeight="12280" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -397,20 +397,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>1</v>
       </c>
@@ -435,8 +435,17 @@
       <c r="I2" s="1">
         <v>43118</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" s="3" customFormat="1" ht="96" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J2" s="1">
+        <v>43122</v>
+      </c>
+      <c r="K2" s="1">
+        <v>43126</v>
+      </c>
+      <c r="L2" s="1">
+        <v>43136</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" s="3" customFormat="1" ht="96" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C3" s="3" t="s">
         <v>3</v>
       </c>
@@ -453,7 +462,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B4">
         <v>0</v>
       </c>
@@ -478,8 +487,17 @@
       <c r="I4">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J4">
+        <v>14</v>
+      </c>
+      <c r="K4">
+        <v>14</v>
+      </c>
+      <c r="L4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B5">
         <v>1</v>
       </c>
@@ -504,8 +522,17 @@
       <c r="I5">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J5">
+        <v>7</v>
+      </c>
+      <c r="K5">
+        <v>7</v>
+      </c>
+      <c r="L5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B6">
         <v>2</v>
       </c>
@@ -530,8 +557,17 @@
       <c r="I6">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J6">
+        <v>6</v>
+      </c>
+      <c r="K6">
+        <v>6</v>
+      </c>
+      <c r="L6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B7">
         <v>3</v>
       </c>
@@ -556,8 +592,17 @@
       <c r="I7">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J7">
+        <v>8</v>
+      </c>
+      <c r="K7">
+        <v>8</v>
+      </c>
+      <c r="L7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B8">
         <v>4</v>
       </c>
@@ -582,8 +627,17 @@
       <c r="I8">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J8">
+        <v>4</v>
+      </c>
+      <c r="K8">
+        <v>4</v>
+      </c>
+      <c r="L8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B9">
         <v>5</v>
       </c>
@@ -608,8 +662,17 @@
       <c r="I9">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J9">
+        <v>4</v>
+      </c>
+      <c r="K9">
+        <v>4</v>
+      </c>
+      <c r="L9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B10">
         <v>6</v>
       </c>
@@ -634,8 +697,17 @@
       <c r="I10">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J10">
+        <v>3</v>
+      </c>
+      <c r="K10">
+        <v>3</v>
+      </c>
+      <c r="L10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B11">
         <v>7</v>
       </c>
@@ -660,8 +732,17 @@
       <c r="I11">
         <v>8</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J11">
+        <v>6</v>
+      </c>
+      <c r="K11">
+        <v>6</v>
+      </c>
+      <c r="L11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B12">
         <v>8</v>
       </c>
@@ -686,8 +767,17 @@
       <c r="I12">
         <v>8</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J12">
+        <v>8</v>
+      </c>
+      <c r="K12">
+        <v>6</v>
+      </c>
+      <c r="L12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B13">
         <v>9</v>
       </c>
@@ -712,8 +802,17 @@
       <c r="I13">
         <v>28</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J13">
+        <v>11</v>
+      </c>
+      <c r="K13">
+        <v>4</v>
+      </c>
+      <c r="L13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B14">
         <v>10</v>
       </c>
@@ -738,8 +837,17 @@
       <c r="I14">
         <v>112</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J14">
+        <v>49</v>
+      </c>
+      <c r="K14">
+        <v>28</v>
+      </c>
+      <c r="L14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B15">
         <v>11</v>
       </c>
@@ -764,8 +872,17 @@
       <c r="I15">
         <v>53</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J15">
+        <v>94</v>
+      </c>
+      <c r="K15">
+        <v>112</v>
+      </c>
+      <c r="L15">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B16">
         <v>12</v>
       </c>
@@ -790,8 +907,17 @@
       <c r="I16">
         <v>3</v>
       </c>
-    </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="J16">
+        <v>45</v>
+      </c>
+      <c r="K16">
+        <v>57</v>
+      </c>
+      <c r="L16">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>0</v>
       </c>
@@ -823,8 +949,20 @@
         <f t="shared" si="0"/>
         <v>8.5482625482625476</v>
       </c>
-    </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="J17" s="2">
+        <f t="shared" ref="J17:K17" si="1">SUMPRODUCT($B$4:$B$16,J4:J16)/SUM(J4:J16)</f>
+        <v>9.1351351351351351</v>
+      </c>
+      <c r="K17" s="2">
+        <f t="shared" si="1"/>
+        <v>9.3397683397683391</v>
+      </c>
+      <c r="L17" s="2">
+        <f t="shared" ref="L17" si="2">SUMPRODUCT($B$4:$B$16,L4:L16)/SUM(L4:L16)</f>
+        <v>9.5598455598455594</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>7</v>
       </c>
@@ -833,27 +971,39 @@
         <v>259</v>
       </c>
       <c r="D18">
-        <f t="shared" ref="D18:G18" si="1">SUM(D4:D16)</f>
+        <f t="shared" ref="D18:G18" si="3">SUM(D4:D16)</f>
         <v>259</v>
       </c>
       <c r="E18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>259</v>
       </c>
       <c r="F18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>259</v>
       </c>
       <c r="G18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>259</v>
       </c>
       <c r="H18">
-        <f t="shared" ref="H18:I18" si="2">SUM(H4:H16)</f>
+        <f t="shared" ref="H18:I18" si="4">SUM(H4:H16)</f>
         <v>259</v>
       </c>
       <c r="I18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
+        <v>259</v>
+      </c>
+      <c r="J18">
+        <f t="shared" ref="J18:K18" si="5">SUM(J4:J16)</f>
+        <v>259</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="5"/>
+        <v>259</v>
+      </c>
+      <c r="L18">
+        <f t="shared" ref="L18" si="6">SUM(L4:L16)</f>
         <v>259</v>
       </c>
     </row>

</xml_diff>